<commit_message>
added sounds specifications for werewolf (sound files are redundantly recorded; not all sounds used)
</commit_message>
<xml_diff>
--- a/concept/sound/vampire_sounds_sheet.xlsx
+++ b/concept/sound/vampire_sounds_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="23480" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>Start</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Vampir erreicht Phase 3 (Alternative)</t>
+  </si>
+  <si>
+    <t>Details</t>
   </si>
 </sst>
 </file>
@@ -286,8 +289,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -317,7 +326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="31">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -330,6 +339,9 @@
     <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -342,6 +354,9 @@
     <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -673,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -698,6 +713,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
@@ -842,6 +860,12 @@
       <c r="B10" t="s">
         <v>33</v>
       </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
       <c r="E10" t="s">
         <v>37</v>
       </c>
@@ -853,6 +877,12 @@
       <c r="B11" t="s">
         <v>35</v>
       </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" t="s">
         <v>37</v>
       </c>
@@ -864,6 +894,12 @@
       <c r="B12" t="s">
         <v>36</v>
       </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
       <c r="E12" t="s">
         <v>37</v>
       </c>
@@ -875,6 +911,12 @@
       <c r="B13" t="s">
         <v>40</v>
       </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
       <c r="E13" t="s">
         <v>37</v>
       </c>
@@ -886,6 +928,12 @@
       <c r="B14" t="s">
         <v>43</v>
       </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" t="s">
         <v>41</v>
       </c>
@@ -897,6 +945,12 @@
       <c r="B15" t="s">
         <v>45</v>
       </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" t="s">
         <v>41</v>
       </c>
@@ -908,6 +962,12 @@
       <c r="B16" t="s">
         <v>47</v>
       </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" t="s">
         <v>41</v>
       </c>
@@ -919,6 +979,12 @@
       <c r="B17" t="s">
         <v>49</v>
       </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
       <c r="E17" t="s">
         <v>41</v>
       </c>
@@ -930,6 +996,12 @@
       <c r="B18" t="s">
         <v>52</v>
       </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" t="s">
         <v>51</v>
       </c>
@@ -941,6 +1013,12 @@
       <c r="B19" t="s">
         <v>54</v>
       </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
       <c r="E19" t="s">
         <v>51</v>
       </c>
@@ -952,6 +1030,12 @@
       <c r="B20" t="s">
         <v>56</v>
       </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
       <c r="E20" t="s">
         <v>51</v>
       </c>
@@ -963,6 +1047,12 @@
       <c r="B21" t="s">
         <v>58</v>
       </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
       <c r="E21" t="s">
         <v>51</v>
       </c>
@@ -974,6 +1064,12 @@
       <c r="B22" t="s">
         <v>59</v>
       </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
       <c r="E22" t="s">
         <v>51</v>
       </c>
@@ -985,6 +1081,12 @@
       <c r="B23" t="s">
         <v>62</v>
       </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
       <c r="E23" t="s">
         <v>63</v>
       </c>
@@ -996,6 +1098,12 @@
       <c r="B24" t="s">
         <v>65</v>
       </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
       <c r="E24" t="s">
         <v>66</v>
       </c>
@@ -1007,6 +1115,12 @@
       <c r="B25" t="s">
         <v>68</v>
       </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
       <c r="E25" t="s">
         <v>23</v>
       </c>
@@ -1017,6 +1131,12 @@
       </c>
       <c r="B26" t="s">
         <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
       </c>
       <c r="E26" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
adjusted vampire sound sheet (Player Death Sound related) and added the sound sheets for DH and Angel
</commit_message>
<xml_diff>
--- a/concept/sound/vampire_sounds_sheet.xlsx
+++ b/concept/sound/vampire_sounds_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23480" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -210,9 +210,6 @@
     <t>02:40.527</t>
   </si>
   <si>
-    <t>Verhöhnen / Auslachen</t>
-  </si>
-  <si>
     <t>02:42.400</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Details</t>
+  </si>
+  <si>
+    <t>Verhöhnen / Auslachen / Vampir gewinnt den Kampf (Death Screen)</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -714,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -816,7 +816,7 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1088,32 +1088,32 @@
         <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
         <v>65</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
         <v>67</v>
-      </c>
-      <c r="B25" t="s">
-        <v>68</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -1127,19 +1127,19 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
         <v>70</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
         <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>